<commit_message>
Add automation tests for Languages and Skills
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Mars.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Mars.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>username</t>
   </si>
@@ -19,29 +19,25 @@
     <t>password</t>
   </si>
   <si>
-    <t>mvpstudio.qa@gmail.com</t>
-  </si>
-  <si>
-    <t>SydneyQa2018</t>
+    <t>dilhaniwas+1@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -67,14 +63,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -130,14 +124,14 @@
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Calibri"/>
-        <a:cs typeface="Calibri"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface="Calibri"/>
-        <a:cs typeface="Calibri"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -293,7 +287,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="48.25"/>
     <col customWidth="1" min="2" max="2" width="12.75"/>
-    <col customWidth="1" min="3" max="26" width="7.63"/>
+    <col customWidth="1" min="3" max="6" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -308,8 +302,8 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+      <c r="B2" s="2">
+        <v>123456.0</v>
       </c>
     </row>
     <row r="3">

</xml_diff>